<commit_message>
added more courses to convertion list
</commit_message>
<xml_diff>
--- a/Leerplanillacupos/data/140823.xlsx
+++ b/Leerplanillacupos/data/140823.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gastonmousques/workspace/ExcelExporter/excelconverter/Leerplanillacupos/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69B85F3-EF84-6E41-92F8-CA8FCFAECA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E109888-137E-6949-BEFB-7231E2FB2149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="760" windowWidth="21600" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2213,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G305"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="13"/>
@@ -9146,12 +9146,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="95c80e47-662b-4bc0-a457-b879d3f3aba4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9410,20 +9412,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="95c80e47-662b-4bc0-a457-b879d3f3aba4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2671E79-D510-48B5-859C-A0DCC874C53A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2CB7EC2-18F2-46C6-A8AA-D895E9A30195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f"/>
+    <ds:schemaRef ds:uri="95c80e47-662b-4bc0-a457-b879d3f3aba4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9448,12 +9451,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2CB7EC2-18F2-46C6-A8AA-D895E9A30195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2671E79-D510-48B5-859C-A0DCC874C53A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7f019ab0-5ffe-43e1-b2f8-62bc369ebe4f"/>
-    <ds:schemaRef ds:uri="95c80e47-662b-4bc0-a457-b879d3f3aba4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>